<commit_message>
fixes joined date employee data
</commit_message>
<xml_diff>
--- a/data/mce_hr.employee.xlsx
+++ b/data/mce_hr.employee.xlsx
@@ -351,12 +351,12 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.85"/>
@@ -427,7 +427,7 @@
         <v>29231</v>
       </c>
       <c r="E2" s="4" t="n">
-        <v>2046</v>
+        <v>38571</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>16</v>
@@ -460,7 +460,7 @@
         <v>28371</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>2046</v>
+        <v>38571</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>23</v>
@@ -493,7 +493,7 @@
         <v>26885</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>2411</v>
+        <v>38936</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>28</v>
@@ -522,7 +522,7 @@
         <v>30393</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>2441</v>
+        <v>38966</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>33</v>
@@ -551,7 +551,7 @@
         <v>28804</v>
       </c>
       <c r="E6" s="4" t="n">
-        <v>2445</v>
+        <v>38970</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>39</v>
@@ -580,7 +580,7 @@
         <v>28893</v>
       </c>
       <c r="E7" s="4" t="n">
-        <v>2559</v>
+        <v>39084</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>45</v>
@@ -609,7 +609,7 @@
         <v>32646</v>
       </c>
       <c r="E8" s="4" t="n">
-        <v>2651</v>
+        <v>39176</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>50</v>
@@ -638,7 +638,7 @@
         <v>31151</v>
       </c>
       <c r="E9" s="4" t="n">
-        <v>2696</v>
+        <v>39221</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>54</v>
@@ -667,7 +667,7 @@
         <v>30682</v>
       </c>
       <c r="E10" s="4" t="n">
-        <v>2938</v>
+        <v>39463</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>59</v>
@@ -696,7 +696,7 @@
         <v>33224</v>
       </c>
       <c r="E11" s="4" t="n">
-        <v>3151</v>
+        <v>39676</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>64</v>

</xml_diff>